<commit_message>
fixes to spike 25
</commit_message>
<xml_diff>
--- a/25c - Spike - Measuring Performance & Optimisations/sample/Results.xlsx
+++ b/25c - Spike - Measuring Performance & Optimisations/sample/Results.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\COS30031-102946740\25c - Spike - Measuring Performance &amp; Optimisations\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A0FAEA-5262-438F-84DA-3A37BF2F10B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B533C852-9A7F-43F0-B395-0D34E475311E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{F38F08C2-2334-4A18-B079-6F7F3B51FA0E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="27" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Test A1</t>
   </si>
@@ -69,6 +73,9 @@
   </si>
   <si>
     <t>Optimized Collision Detection</t>
+  </si>
+  <si>
+    <t>Sum of Loops</t>
   </si>
 </sst>
 </file>
@@ -112,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -123,9 +130,8 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -141,6 +147,1348 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Results.xlsx]Sheet2!PivotTable21</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Sum of Loops/Second by Test Name</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$4:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Optimized Collision Detection</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test A1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test A2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test B</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test C</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Test D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>114690877</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55260450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96203608</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>102352808</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>121145867</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>122458782</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-13A7-4FB5-937B-AF33AD3AEB49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="939348959"/>
+        <c:axId val="939350879"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="939348959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="939350879"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="939350879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="939348959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>292893</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330993</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F380779-578F-4E2F-0CD1-F15CB4B80D1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ben" refreshedDate="45594.428354629628" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="12" xr:uid="{0B5C87AA-DE7C-44F8-891F-074D1B52B16D}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:E13" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Test Name" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Test A1"/>
+        <s v="Test A2"/>
+        <s v="Test B"/>
+        <s v="Test C"/>
+        <s v="Test D"/>
+        <s v="Optimized Collision Detection"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Loops" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="26231991" maxValue="61229391"/>
+    </cacheField>
+    <cacheField name="Time (ms)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10000" maxValue="10000"/>
+    </cacheField>
+    <cacheField name="Loops/Second" numFmtId="11">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2623200" maxValue="6122940"/>
+    </cacheField>
+    <cacheField name="Number of Boxes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="2"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="12">
+  <r>
+    <x v="0"/>
+    <n v="26231991"/>
+    <n v="10000"/>
+    <n v="2623200"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="46687462"/>
+    <n v="10000"/>
+    <n v="4668750"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="49272443"/>
+    <n v="10000"/>
+    <n v="4927240"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="60327791"/>
+    <n v="10000"/>
+    <n v="6032780"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="61229391"/>
+    <n v="10000"/>
+    <n v="6122940"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="29028459"/>
+    <n v="10000"/>
+    <n v="2902850"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="49516146"/>
+    <n v="10000"/>
+    <n v="4951610"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="53080365"/>
+    <n v="10000"/>
+    <n v="5308040"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="60818076"/>
+    <n v="10000"/>
+    <n v="6081810"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="61229391"/>
+    <n v="10000"/>
+    <n v="6122940"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="55652600"/>
+    <n v="10000"/>
+    <n v="5565260"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="59038277"/>
+    <n v="10000"/>
+    <n v="5903830"/>
+    <n v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3327E82D-2123-4899-A76D-5EF78C32DA69}" name="PivotTable21" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="15">
+  <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="5"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+      </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" numFmtId="11" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Loops" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="11" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="12" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,11 +1807,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B00175-EF9A-4B0A-AAFB-341A760192B4}">
+  <dimension ref="A3:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5">
+        <v>114690877</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5">
+        <v>55260450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <v>96203608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5">
+        <v>102352808</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5">
+        <v>121145867</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5">
+        <v>122458782</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31A795A-CC44-4690-8FAC-60BDB54289B4}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -497,13 +1921,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>602</v>
+        <v>26231991</v>
       </c>
       <c r="C2" s="1">
-        <v>10036</v>
-      </c>
-      <c r="D2" s="1">
-        <v>59.984099999999998</v>
+        <v>10000</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2623200</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
@@ -514,13 +1938,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>602</v>
+        <v>46687462</v>
       </c>
       <c r="C3" s="1">
-        <v>10025</v>
-      </c>
-      <c r="D3" s="1">
-        <v>60.049900000000001</v>
+        <v>10000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4668750</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -531,13 +1955,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>601</v>
+        <v>49272443</v>
       </c>
       <c r="C4" s="1">
-        <v>10026</v>
-      </c>
-      <c r="D4" s="1">
-        <v>59.944099999999999</v>
+        <v>10000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4927240</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -548,13 +1972,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>601</v>
+        <v>60327791</v>
       </c>
       <c r="C5" s="1">
-        <v>10023</v>
-      </c>
-      <c r="D5" s="1">
-        <v>59.9621</v>
+        <v>10000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6032780</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -565,13 +1989,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>601</v>
+        <v>61229391</v>
       </c>
       <c r="C6" s="1">
-        <v>10024</v>
-      </c>
-      <c r="D6" s="1">
-        <v>59.956099999999999</v>
+        <v>10000</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6122940</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -582,13 +2006,13 @@
         <v>0</v>
       </c>
       <c r="B7" s="1">
-        <v>601</v>
+        <v>29028459</v>
       </c>
       <c r="C7" s="1">
-        <v>10021</v>
-      </c>
-      <c r="D7" s="1">
-        <v>59.9741</v>
+        <v>10000</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2902850</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -599,13 +2023,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <v>600</v>
+        <v>49516146</v>
       </c>
       <c r="C8" s="1">
-        <v>10021</v>
-      </c>
-      <c r="D8" s="1">
-        <v>59.874299999999998</v>
+        <v>10000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4951610</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -616,13 +2040,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1">
-        <v>601</v>
+        <v>53080365</v>
       </c>
       <c r="C9" s="1">
-        <v>10025</v>
-      </c>
-      <c r="D9" s="1">
-        <v>59.950099999999999</v>
+        <v>10000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5308040</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -633,13 +2057,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>601</v>
+        <v>60818076</v>
       </c>
       <c r="C10" s="1">
-        <v>10024</v>
-      </c>
-      <c r="D10" s="1">
-        <v>59.956099999999999</v>
+        <v>10000</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6081810</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -650,20 +2074,20 @@
         <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>602</v>
+        <v>61229391</v>
       </c>
       <c r="C11" s="1">
-        <v>10032</v>
-      </c>
-      <c r="D11" s="1">
-        <v>60.008000000000003</v>
+        <v>10000</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6122940</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -680,7 +2104,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1">

</xml_diff>